<commit_message>
adding the latest file
</commit_message>
<xml_diff>
--- a/Corona_database_extract.xlsx
+++ b/Corona_database_extract.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3151"/>
+  <dimension ref="A1:H3186"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -89948,6 +89948,1056 @@
         <v>11</v>
       </c>
     </row>
+    <row r="3152">
+      <c r="A3152" t="inlineStr">
+        <is>
+          <t>Andaman and Nicobar Islands</t>
+        </is>
+      </c>
+      <c r="B3152" t="n">
+        <v>59</v>
+      </c>
+      <c r="C3152" t="n">
+        <v>43</v>
+      </c>
+      <c r="D3152" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3152" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3152" t="n">
+        <v>12</v>
+      </c>
+      <c r="G3152" t="n">
+        <v>7</v>
+      </c>
+      <c r="H3152" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3153">
+      <c r="A3153" t="inlineStr">
+        <is>
+          <t>Andhra Pradesh</t>
+        </is>
+      </c>
+      <c r="B3153" t="n">
+        <v>10884</v>
+      </c>
+      <c r="C3153" t="n">
+        <v>4988</v>
+      </c>
+      <c r="D3153" t="n">
+        <v>136</v>
+      </c>
+      <c r="E3153" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3153" t="n">
+        <v>2432</v>
+      </c>
+      <c r="G3153" t="n">
+        <v>877</v>
+      </c>
+      <c r="H3153" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3154">
+      <c r="A3154" t="inlineStr">
+        <is>
+          <t>Arunachal Pradesh</t>
+        </is>
+      </c>
+      <c r="B3154" t="n">
+        <v>160</v>
+      </c>
+      <c r="C3154" t="n">
+        <v>38</v>
+      </c>
+      <c r="D3154" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3154" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3154" t="n">
+        <v>25</v>
+      </c>
+      <c r="G3154" t="n">
+        <v>24</v>
+      </c>
+      <c r="H3154" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3155">
+      <c r="A3155" t="inlineStr">
+        <is>
+          <t>Assam</t>
+        </is>
+      </c>
+      <c r="B3155" t="n">
+        <v>6321</v>
+      </c>
+      <c r="C3155" t="n">
+        <v>4033</v>
+      </c>
+      <c r="D3155" t="n">
+        <v>9</v>
+      </c>
+      <c r="E3155" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3155" t="n">
+        <v>1417</v>
+      </c>
+      <c r="G3155" t="n">
+        <v>994</v>
+      </c>
+      <c r="H3155" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3156">
+      <c r="A3156" t="inlineStr">
+        <is>
+          <t>Bihar</t>
+        </is>
+      </c>
+      <c r="B3156" t="n">
+        <v>8473</v>
+      </c>
+      <c r="C3156" t="n">
+        <v>6441</v>
+      </c>
+      <c r="D3156" t="n">
+        <v>57</v>
+      </c>
+      <c r="E3156" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3156" t="n">
+        <v>940</v>
+      </c>
+      <c r="G3156" t="n">
+        <v>912</v>
+      </c>
+      <c r="H3156" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3157">
+      <c r="A3157" t="inlineStr">
+        <is>
+          <t>Chandigarh</t>
+        </is>
+      </c>
+      <c r="B3157" t="n">
+        <v>423</v>
+      </c>
+      <c r="C3157" t="n">
+        <v>329</v>
+      </c>
+      <c r="D3157" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3157" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3157" t="n">
+        <v>19</v>
+      </c>
+      <c r="G3157" t="n">
+        <v>13</v>
+      </c>
+      <c r="H3157" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3158">
+      <c r="A3158" t="inlineStr">
+        <is>
+          <t>Chhattisgarh</t>
+        </is>
+      </c>
+      <c r="B3158" t="n">
+        <v>2452</v>
+      </c>
+      <c r="C3158" t="n">
+        <v>1755</v>
+      </c>
+      <c r="D3158" t="n">
+        <v>12</v>
+      </c>
+      <c r="E3158" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3158" t="n">
+        <v>411</v>
+      </c>
+      <c r="G3158" t="n">
+        <v>361</v>
+      </c>
+      <c r="H3158" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3159">
+      <c r="A3159" t="inlineStr">
+        <is>
+          <t>Dadra and Nagar Haveli and Daman and Diu</t>
+        </is>
+      </c>
+      <c r="B3159" t="n">
+        <v>155</v>
+      </c>
+      <c r="C3159" t="n">
+        <v>32</v>
+      </c>
+      <c r="D3159" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3159" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3159" t="n">
+        <v>87</v>
+      </c>
+      <c r="G3159" t="n">
+        <v>6</v>
+      </c>
+      <c r="H3159" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3160">
+      <c r="A3160" t="inlineStr">
+        <is>
+          <t>Delhi</t>
+        </is>
+      </c>
+      <c r="B3160" t="n">
+        <v>73780</v>
+      </c>
+      <c r="C3160" t="n">
+        <v>44765</v>
+      </c>
+      <c r="D3160" t="n">
+        <v>2429</v>
+      </c>
+      <c r="E3160" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3160" t="n">
+        <v>17034</v>
+      </c>
+      <c r="G3160" t="n">
+        <v>13471</v>
+      </c>
+      <c r="H3160" t="n">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="3161">
+      <c r="A3161" t="inlineStr">
+        <is>
+          <t>Goa</t>
+        </is>
+      </c>
+      <c r="B3161" t="n">
+        <v>995</v>
+      </c>
+      <c r="C3161" t="n">
+        <v>335</v>
+      </c>
+      <c r="D3161" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3161" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3161" t="n">
+        <v>241</v>
+      </c>
+      <c r="G3161" t="n">
+        <v>206</v>
+      </c>
+      <c r="H3161" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3162">
+      <c r="A3162" t="inlineStr">
+        <is>
+          <t>Gujarat</t>
+        </is>
+      </c>
+      <c r="B3162" t="n">
+        <v>29520</v>
+      </c>
+      <c r="C3162" t="n">
+        <v>21498</v>
+      </c>
+      <c r="D3162" t="n">
+        <v>1753</v>
+      </c>
+      <c r="E3162" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3162" t="n">
+        <v>2840</v>
+      </c>
+      <c r="G3162" t="n">
+        <v>2804</v>
+      </c>
+      <c r="H3162" t="n">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3163">
+      <c r="A3163" t="inlineStr">
+        <is>
+          <t>Haryana</t>
+        </is>
+      </c>
+      <c r="B3163" t="n">
+        <v>12463</v>
+      </c>
+      <c r="C3163" t="n">
+        <v>7380</v>
+      </c>
+      <c r="D3163" t="n">
+        <v>198</v>
+      </c>
+      <c r="E3163" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3163" t="n">
+        <v>2240</v>
+      </c>
+      <c r="G3163" t="n">
+        <v>2252</v>
+      </c>
+      <c r="H3163" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3164">
+      <c r="A3164" t="inlineStr">
+        <is>
+          <t>Himachal Pradesh</t>
+        </is>
+      </c>
+      <c r="B3164" t="n">
+        <v>839</v>
+      </c>
+      <c r="C3164" t="n">
+        <v>477</v>
+      </c>
+      <c r="D3164" t="n">
+        <v>9</v>
+      </c>
+      <c r="E3164" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3164" t="n">
+        <v>183</v>
+      </c>
+      <c r="G3164" t="n">
+        <v>64</v>
+      </c>
+      <c r="H3164" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3165">
+      <c r="A3165" t="inlineStr">
+        <is>
+          <t>Jammu and Kashmir</t>
+        </is>
+      </c>
+      <c r="B3165" t="n">
+        <v>6549</v>
+      </c>
+      <c r="C3165" t="n">
+        <v>3967</v>
+      </c>
+      <c r="D3165" t="n">
+        <v>90</v>
+      </c>
+      <c r="E3165" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3165" t="n">
+        <v>715</v>
+      </c>
+      <c r="G3165" t="n">
+        <v>631</v>
+      </c>
+      <c r="H3165" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3166">
+      <c r="A3166" t="inlineStr">
+        <is>
+          <t>Jharkhand</t>
+        </is>
+      </c>
+      <c r="B3166" t="n">
+        <v>2262</v>
+      </c>
+      <c r="C3166" t="n">
+        <v>1605</v>
+      </c>
+      <c r="D3166" t="n">
+        <v>12</v>
+      </c>
+      <c r="E3166" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3166" t="n">
+        <v>297</v>
+      </c>
+      <c r="G3166" t="n">
+        <v>270</v>
+      </c>
+      <c r="H3166" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3167">
+      <c r="A3167" t="inlineStr">
+        <is>
+          <t>Karnataka</t>
+        </is>
+      </c>
+      <c r="B3167" t="n">
+        <v>10560</v>
+      </c>
+      <c r="C3167" t="n">
+        <v>6670</v>
+      </c>
+      <c r="D3167" t="n">
+        <v>170</v>
+      </c>
+      <c r="E3167" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3167" t="n">
+        <v>1863</v>
+      </c>
+      <c r="G3167" t="n">
+        <v>1279</v>
+      </c>
+      <c r="H3167" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3168">
+      <c r="A3168" t="inlineStr">
+        <is>
+          <t>Kerala</t>
+        </is>
+      </c>
+      <c r="B3168" t="n">
+        <v>3726</v>
+      </c>
+      <c r="C3168" t="n">
+        <v>1943</v>
+      </c>
+      <c r="D3168" t="n">
+        <v>22</v>
+      </c>
+      <c r="E3168" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3168" t="n">
+        <v>687</v>
+      </c>
+      <c r="G3168" t="n">
+        <v>375</v>
+      </c>
+      <c r="H3168" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3169">
+      <c r="A3169" t="inlineStr">
+        <is>
+          <t>Ladakh</t>
+        </is>
+      </c>
+      <c r="B3169" t="n">
+        <v>941</v>
+      </c>
+      <c r="C3169" t="n">
+        <v>358</v>
+      </c>
+      <c r="D3169" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3169" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3169" t="n">
+        <v>105</v>
+      </c>
+      <c r="G3169" t="n">
+        <v>241</v>
+      </c>
+      <c r="H3169" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3170">
+      <c r="A3170" t="inlineStr">
+        <is>
+          <t>Madhya Pradesh</t>
+        </is>
+      </c>
+      <c r="B3170" t="n">
+        <v>12596</v>
+      </c>
+      <c r="C3170" t="n">
+        <v>9619</v>
+      </c>
+      <c r="D3170" t="n">
+        <v>542</v>
+      </c>
+      <c r="E3170" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3170" t="n">
+        <v>872</v>
+      </c>
+      <c r="G3170" t="n">
+        <v>739</v>
+      </c>
+      <c r="H3170" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3171">
+      <c r="A3171" t="inlineStr">
+        <is>
+          <t>Maharashtra</t>
+        </is>
+      </c>
+      <c r="B3171" t="n">
+        <v>147741</v>
+      </c>
+      <c r="C3171" t="n">
+        <v>77453</v>
+      </c>
+      <c r="D3171" t="n">
+        <v>6931</v>
+      </c>
+      <c r="E3171" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3171" t="n">
+        <v>19536</v>
+      </c>
+      <c r="G3171" t="n">
+        <v>13300</v>
+      </c>
+      <c r="H3171" t="n">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="3172">
+      <c r="A3172" t="inlineStr">
+        <is>
+          <t>Manipur</t>
+        </is>
+      </c>
+      <c r="B3172" t="n">
+        <v>1056</v>
+      </c>
+      <c r="C3172" t="n">
+        <v>354</v>
+      </c>
+      <c r="D3172" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3172" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3172" t="n">
+        <v>279</v>
+      </c>
+      <c r="G3172" t="n">
+        <v>122</v>
+      </c>
+      <c r="H3172" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3173">
+      <c r="A3173" t="inlineStr">
+        <is>
+          <t>Meghalaya</t>
+        </is>
+      </c>
+      <c r="B3173" t="n">
+        <v>46</v>
+      </c>
+      <c r="C3173" t="n">
+        <v>42</v>
+      </c>
+      <c r="D3173" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3173" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3173" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3173" t="n">
+        <v>9</v>
+      </c>
+      <c r="H3173" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3174">
+      <c r="A3174" t="inlineStr">
+        <is>
+          <t>Mizoram</t>
+        </is>
+      </c>
+      <c r="B3174" t="n">
+        <v>145</v>
+      </c>
+      <c r="C3174" t="n">
+        <v>30</v>
+      </c>
+      <c r="D3174" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3174" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3174" t="n">
+        <v>5</v>
+      </c>
+      <c r="G3174" t="n">
+        <v>21</v>
+      </c>
+      <c r="H3174" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3175">
+      <c r="A3175" t="inlineStr">
+        <is>
+          <t>Nagaland</t>
+        </is>
+      </c>
+      <c r="B3175" t="n">
+        <v>355</v>
+      </c>
+      <c r="C3175" t="n">
+        <v>160</v>
+      </c>
+      <c r="D3175" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3175" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3175" t="n">
+        <v>154</v>
+      </c>
+      <c r="G3175" t="n">
+        <v>22</v>
+      </c>
+      <c r="H3175" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3176">
+      <c r="A3176" t="inlineStr">
+        <is>
+          <t>Odisha</t>
+        </is>
+      </c>
+      <c r="B3176" t="n">
+        <v>5962</v>
+      </c>
+      <c r="C3176" t="n">
+        <v>4291</v>
+      </c>
+      <c r="D3176" t="n">
+        <v>17</v>
+      </c>
+      <c r="E3176" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3176" t="n">
+        <v>1106</v>
+      </c>
+      <c r="G3176" t="n">
+        <v>757</v>
+      </c>
+      <c r="H3176" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3177">
+      <c r="A3177" t="inlineStr">
+        <is>
+          <t>Puducherry</t>
+        </is>
+      </c>
+      <c r="B3177" t="n">
+        <v>502</v>
+      </c>
+      <c r="C3177" t="n">
+        <v>187</v>
+      </c>
+      <c r="D3177" t="n">
+        <v>9</v>
+      </c>
+      <c r="E3177" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3177" t="n">
+        <v>216</v>
+      </c>
+      <c r="G3177" t="n">
+        <v>69</v>
+      </c>
+      <c r="H3177" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3178">
+      <c r="A3178" t="inlineStr">
+        <is>
+          <t>Punjab</t>
+        </is>
+      </c>
+      <c r="B3178" t="n">
+        <v>4769</v>
+      </c>
+      <c r="C3178" t="n">
+        <v>3192</v>
+      </c>
+      <c r="D3178" t="n">
+        <v>120</v>
+      </c>
+      <c r="E3178" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3178" t="n">
+        <v>817</v>
+      </c>
+      <c r="G3178" t="n">
+        <v>514</v>
+      </c>
+      <c r="H3178" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3179">
+      <c r="A3179" t="inlineStr">
+        <is>
+          <t>Rajasthan</t>
+        </is>
+      </c>
+      <c r="B3179" t="n">
+        <v>16296</v>
+      </c>
+      <c r="C3179" t="n">
+        <v>12840</v>
+      </c>
+      <c r="D3179" t="n">
+        <v>379</v>
+      </c>
+      <c r="E3179" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3179" t="n">
+        <v>1760</v>
+      </c>
+      <c r="G3179" t="n">
+        <v>1566</v>
+      </c>
+      <c r="H3179" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3180">
+      <c r="A3180" t="inlineStr">
+        <is>
+          <t>Sikkim</t>
+        </is>
+      </c>
+      <c r="B3180" t="n">
+        <v>85</v>
+      </c>
+      <c r="C3180" t="n">
+        <v>39</v>
+      </c>
+      <c r="D3180" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3180" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3180" t="n">
+        <v>15</v>
+      </c>
+      <c r="G3180" t="n">
+        <v>14</v>
+      </c>
+      <c r="H3180" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3181">
+      <c r="A3181" t="inlineStr">
+        <is>
+          <t>Tamil Nadu</t>
+        </is>
+      </c>
+      <c r="B3181" t="n">
+        <v>70977</v>
+      </c>
+      <c r="C3181" t="n">
+        <v>39999</v>
+      </c>
+      <c r="D3181" t="n">
+        <v>911</v>
+      </c>
+      <c r="E3181" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3181" t="n">
+        <v>14132</v>
+      </c>
+      <c r="G3181" t="n">
+        <v>8683</v>
+      </c>
+      <c r="H3181" t="n">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="3182">
+      <c r="A3182" t="inlineStr">
+        <is>
+          <t>Telangana</t>
+        </is>
+      </c>
+      <c r="B3182" t="n">
+        <v>11364</v>
+      </c>
+      <c r="C3182" t="n">
+        <v>4688</v>
+      </c>
+      <c r="D3182" t="n">
+        <v>230</v>
+      </c>
+      <c r="E3182" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3182" t="n">
+        <v>4292</v>
+      </c>
+      <c r="G3182" t="n">
+        <v>1182</v>
+      </c>
+      <c r="H3182" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3183">
+      <c r="A3183" t="inlineStr">
+        <is>
+          <t>Tripura</t>
+        </is>
+      </c>
+      <c r="B3183" t="n">
+        <v>1290</v>
+      </c>
+      <c r="C3183" t="n">
+        <v>1019</v>
+      </c>
+      <c r="D3183" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3183" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3183" t="n">
+        <v>104</v>
+      </c>
+      <c r="G3183" t="n">
+        <v>339</v>
+      </c>
+      <c r="H3183" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3184">
+      <c r="A3184" t="inlineStr">
+        <is>
+          <t>Uttarakhand</t>
+        </is>
+      </c>
+      <c r="B3184" t="n">
+        <v>2691</v>
+      </c>
+      <c r="C3184" t="n">
+        <v>1758</v>
+      </c>
+      <c r="D3184" t="n">
+        <v>36</v>
+      </c>
+      <c r="E3184" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3184" t="n">
+        <v>390</v>
+      </c>
+      <c r="G3184" t="n">
+        <v>308</v>
+      </c>
+      <c r="H3184" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3185">
+      <c r="A3185" t="inlineStr">
+        <is>
+          <t>Uttar Pradesh</t>
+        </is>
+      </c>
+      <c r="B3185" t="n">
+        <v>20193</v>
+      </c>
+      <c r="C3185" t="n">
+        <v>13119</v>
+      </c>
+      <c r="D3185" t="n">
+        <v>611</v>
+      </c>
+      <c r="E3185" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3185" t="n">
+        <v>3599</v>
+      </c>
+      <c r="G3185" t="n">
+        <v>3124</v>
+      </c>
+      <c r="H3185" t="n">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3186">
+      <c r="A3186" t="inlineStr">
+        <is>
+          <t>West Bengal</t>
+        </is>
+      </c>
+      <c r="B3186" t="n">
+        <v>15648</v>
+      </c>
+      <c r="C3186" t="n">
+        <v>10190</v>
+      </c>
+      <c r="D3186" t="n">
+        <v>606</v>
+      </c>
+      <c r="E3186" t="inlineStr">
+        <is>
+          <t>26-06-2020</t>
+        </is>
+      </c>
+      <c r="F3186" t="n">
+        <v>2117</v>
+      </c>
+      <c r="G3186" t="n">
+        <v>2325</v>
+      </c>
+      <c r="H3186" t="n">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>